<commit_message>
Changes to pairs matrix
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="pairs" sheetId="1" r:id="rId1"/>
@@ -890,7 +890,7 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="28">
     <dxf>
       <font>
         <color auto="1"/>
@@ -913,21 +913,21 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -993,26 +993,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
       <fill>
@@ -1028,66 +1008,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1533,7 +1453,7 @@
   <dimension ref="A1:AU49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AM37" sqref="AM37"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1817,7 @@
       <c r="O3" s="4">
         <v>0</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="17">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
@@ -1907,16 +1827,16 @@
         <v>0</v>
       </c>
       <c r="S3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="4">
         <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W3" s="4">
         <v>0</v>
@@ -1925,13 +1845,13 @@
         <v>0</v>
       </c>
       <c r="Y3" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="4">
         <v>2092</v>
       </c>
       <c r="AA3" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="4">
         <v>0</v>
@@ -1939,17 +1859,17 @@
       <c r="AC3" s="4">
         <v>0</v>
       </c>
-      <c r="AD3" s="4">
-        <v>2</v>
+      <c r="AD3" s="17">
+        <v>1</v>
       </c>
       <c r="AE3" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="4">
         <v>1</v>
@@ -1958,7 +1878,7 @@
         <v>2</v>
       </c>
       <c r="AJ3" s="4">
-        <v>10414</v>
+        <v>10427</v>
       </c>
       <c r="AK3" s="4">
         <v>5</v>
@@ -1985,15 +1905,15 @@
         <v>0</v>
       </c>
       <c r="AS3" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AT3" s="3">
         <f t="shared" ref="AT3:AT45" si="0">SUM(B3:AS3)</f>
-        <v>12605</v>
+        <v>12594</v>
       </c>
       <c r="AU3" s="3">
         <f t="shared" ref="AU3:AU45" si="1">COUNTIF(B3:AS3, 0)</f>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
@@ -2094,7 +2014,7 @@
         <v>6</v>
       </c>
       <c r="AG4" s="4">
-        <v>2316</v>
+        <v>2317</v>
       </c>
       <c r="AH4" s="4">
         <v>0</v>
@@ -2134,7 +2054,7 @@
       </c>
       <c r="AT4" s="3">
         <f t="shared" si="0"/>
-        <v>7459</v>
+        <v>7460</v>
       </c>
       <c r="AU4" s="3">
         <f t="shared" si="1"/>
@@ -2215,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="Y5" s="4">
-        <v>2765</v>
+        <v>2766</v>
       </c>
       <c r="Z5" s="4">
         <v>2122</v>
@@ -2233,7 +2153,7 @@
         <v>4445</v>
       </c>
       <c r="AE5" s="4">
-        <v>20362</v>
+        <v>20364</v>
       </c>
       <c r="AF5" s="4">
         <v>10147</v>
@@ -2279,7 +2199,7 @@
       </c>
       <c r="AT5" s="3">
         <f t="shared" si="0"/>
-        <v>131161</v>
+        <v>131164</v>
       </c>
       <c r="AU5" s="3">
         <f t="shared" si="1"/>
@@ -2819,7 +2739,7 @@
         <v>2001</v>
       </c>
       <c r="AG9" s="4">
-        <v>7578</v>
+        <v>7583</v>
       </c>
       <c r="AH9" s="4">
         <v>4</v>
@@ -2859,7 +2779,7 @@
       </c>
       <c r="AT9" s="3">
         <f t="shared" si="0"/>
-        <v>41321</v>
+        <v>41326</v>
       </c>
       <c r="AU9" s="3">
         <f t="shared" si="1"/>
@@ -3178,7 +3098,7 @@
       <c r="G12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="4">
         <v>0</v>
       </c>
       <c r="I12" s="4">
@@ -3309,7 +3229,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -3387,7 +3307,7 @@
         <v>19</v>
       </c>
       <c r="AC13" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD13" s="4">
         <v>20</v>
@@ -3443,7 +3363,7 @@
       </c>
       <c r="AU13" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
@@ -4206,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" s="4">
         <v>0</v>
@@ -4309,7 +4229,7 @@
       </c>
       <c r="AT19" s="3">
         <f t="shared" si="0"/>
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="AU19" s="3">
         <f t="shared" si="1"/>
@@ -4759,13 +4679,13 @@
         <v>492</v>
       </c>
       <c r="C23" s="4">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D23" s="4">
         <v>2</v>
       </c>
       <c r="E23" s="4">
-        <v>2633</v>
+        <v>2634</v>
       </c>
       <c r="F23" s="4">
         <v>303</v>
@@ -5194,7 +5114,7 @@
         <v>1019</v>
       </c>
       <c r="C26" s="4">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D26" s="4">
         <v>2</v>
@@ -5278,7 +5198,7 @@
         <v>4</v>
       </c>
       <c r="AE26" s="4">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AF26" s="4">
         <v>185</v>
@@ -5629,7 +5549,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="4">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="4">
         <v>50</v>
@@ -5647,7 +5567,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="4">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="J29" s="4">
         <v>49</v>
@@ -5759,7 +5679,7 @@
       </c>
       <c r="AT29" s="3">
         <f t="shared" si="0"/>
-        <v>9480</v>
+        <v>9484</v>
       </c>
       <c r="AU29" s="3">
         <f t="shared" si="1"/>
@@ -6064,13 +5984,13 @@
         <v>2578</v>
       </c>
       <c r="C32" s="4">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
       </c>
       <c r="E32" s="4">
-        <v>9047</v>
+        <v>9048</v>
       </c>
       <c r="F32" s="4">
         <v>2775</v>
@@ -6398,7 +6318,7 @@
       <c r="Q34" s="4">
         <v>2</v>
       </c>
-      <c r="R34" s="17">
+      <c r="R34" s="4">
         <v>0</v>
       </c>
       <c r="S34" s="4">
@@ -6505,7 +6425,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="4">
-        <v>6476</v>
+        <v>6475</v>
       </c>
       <c r="F35" s="4">
         <v>2972</v>
@@ -6598,7 +6518,7 @@
         <v>11</v>
       </c>
       <c r="AJ35" s="4">
-        <v>4975</v>
+        <v>4976</v>
       </c>
       <c r="AK35" s="4">
         <v>578</v>
@@ -6650,7 +6570,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <v>11768</v>
+        <v>11769</v>
       </c>
       <c r="F36" s="4">
         <v>3617</v>
@@ -6698,10 +6618,10 @@
         <v>3291</v>
       </c>
       <c r="U36" s="4">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="V36" s="4">
-        <v>4712</v>
+        <v>4717</v>
       </c>
       <c r="W36" s="4">
         <v>810</v>
@@ -6710,13 +6630,13 @@
         <v>4939</v>
       </c>
       <c r="Y36" s="4">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="Z36" s="4">
         <v>905</v>
       </c>
       <c r="AA36" s="4">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AB36" s="4">
         <v>12087</v>
@@ -6725,16 +6645,16 @@
         <v>58</v>
       </c>
       <c r="AD36" s="4">
-        <v>2770</v>
+        <v>2771</v>
       </c>
       <c r="AE36" s="4">
         <v>1305</v>
       </c>
       <c r="AF36" s="4">
-        <v>2725</v>
+        <v>2726</v>
       </c>
       <c r="AG36" s="4">
-        <v>3198</v>
+        <v>3199</v>
       </c>
       <c r="AH36" s="4">
         <v>4621</v>
@@ -6774,7 +6694,7 @@
       </c>
       <c r="AT36" s="3">
         <f t="shared" si="0"/>
-        <v>95694</v>
+        <v>95708</v>
       </c>
       <c r="AU36" s="3">
         <f t="shared" si="1"/>
@@ -6789,13 +6709,13 @@
         <v>1262</v>
       </c>
       <c r="C37" s="4">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D37" s="4">
         <v>2</v>
       </c>
       <c r="E37" s="4">
-        <v>6826</v>
+        <v>6828</v>
       </c>
       <c r="F37" s="4">
         <v>1186</v>
@@ -7949,13 +7869,13 @@
         <v>194</v>
       </c>
       <c r="C45" s="10">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D45" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E45" s="10">
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="F45" s="10">
         <v>296</v>
@@ -7976,7 +7896,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="10">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M45" s="10">
         <v>4</v>
@@ -8039,7 +7959,7 @@
         <v>424</v>
       </c>
       <c r="AG45" s="10">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AH45" s="10">
         <v>330</v>
@@ -8079,7 +7999,7 @@
       </c>
       <c r="AT45" s="3">
         <f t="shared" si="0"/>
-        <v>8549</v>
+        <v>8550</v>
       </c>
       <c r="AU45" s="3">
         <f t="shared" si="1"/>
@@ -8093,15 +8013,15 @@
       </c>
       <c r="C46" s="3">
         <f t="shared" ref="C46:AT46" si="2">SUM(C2:C45)</f>
-        <v>11679</v>
+        <v>11668</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" si="2"/>
-        <v>7546</v>
+        <v>7547</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" si="2"/>
-        <v>131507</v>
+        <v>131510</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="2"/>
@@ -8117,7 +8037,7 @@
       </c>
       <c r="I46" s="3">
         <f t="shared" si="2"/>
-        <v>37488</v>
+        <v>37493</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" si="2"/>
@@ -8157,7 +8077,7 @@
       </c>
       <c r="S46" s="3">
         <f t="shared" si="2"/>
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="T46" s="3">
         <f t="shared" si="2"/>
@@ -8197,7 +8117,7 @@
       </c>
       <c r="AC46" s="3">
         <f t="shared" si="2"/>
-        <v>7431</v>
+        <v>7435</v>
       </c>
       <c r="AD46" s="3">
         <f t="shared" si="2"/>
@@ -8225,7 +8145,7 @@
       </c>
       <c r="AJ46" s="3">
         <f t="shared" si="2"/>
-        <v>109761</v>
+        <v>109775</v>
       </c>
       <c r="AK46" s="3">
         <f t="shared" si="2"/>
@@ -8261,11 +8181,11 @@
       </c>
       <c r="AS46" s="3">
         <f t="shared" si="2"/>
-        <v>13046</v>
+        <v>13047</v>
       </c>
       <c r="AT46" s="12">
         <f t="shared" si="2"/>
-        <v>1227030</v>
+        <v>1227046</v>
       </c>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.25">
@@ -8342,7 +8262,7 @@
       </c>
       <c r="S47" s="3">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T47" s="3">
         <f t="shared" si="3"/>
@@ -8350,11 +8270,11 @@
       </c>
       <c r="U47" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V47" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W47" s="3">
         <f t="shared" si="3"/>
@@ -8366,7 +8286,7 @@
       </c>
       <c r="Y47" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z47" s="3">
         <f t="shared" si="3"/>
@@ -8374,7 +8294,7 @@
       </c>
       <c r="AA47" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB47" s="3">
         <f t="shared" si="3"/>
@@ -8382,7 +8302,7 @@
       </c>
       <c r="AC47" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD47" s="3">
         <f t="shared" si="3"/>
@@ -8390,15 +8310,15 @@
       </c>
       <c r="AE47" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF47" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG47" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH47" s="3">
         <f t="shared" si="3"/>
@@ -8450,7 +8370,7 @@
       </c>
       <c r="AU47" s="14">
         <f>SUM(AU2:AU45)</f>
-        <v>431</v>
+        <v>438</v>
       </c>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.25">
@@ -8465,25 +8385,43 @@
       </c>
       <c r="AU49" s="23">
         <f>AU47/AU48</f>
-        <v>0.22262396694214875</v>
+        <v>0.2262396694214876</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AS5 B10:Q10 B9 B2:D2 F2:AS2 B8:F8 B7 D7:E7 H8:AS9 B6:D6 G6:AS6 D9:E9 B12:G12 C11:AS11 B16:AS17 C14:G14 B22:AS23 C19:Q19 B45:Q45 C43:AS43 B25:Q27 C24:G24 B44:H44 L44:N44 B42:AS42 B40:J40 L40:AS40 B36:AS36 B34:J34 L34:Q34 B20:J20 L20:AS20 C13:E13 G13:I13 I12:AS12 I14:Q14 B32:Q32 B31:G31 I31:Q31 B33:G33 I33:Q33 G7 I7:AS7 B18:E18 G18:H18 J18 L18:AS18 L13:M13 I24:AS24 B29:Q30 B28:J28 L28:AS28 B15:Q15 S14:AS15 S19:AS19 B21:Q21 S21:AS21 S25:AS27 S10:AS10 B35:Q35 S29:AS35 B37:Q39 S37:AS39 B41:Q41 S41:AS41 S45:AS45 J44 P44:R44 T44 W44:X44 AA44 AD44 AH44 AJ44 AM44:AN44 AP44:AR44 O13:T13 V13:X13 AC13:AS13">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+  <conditionalFormatting sqref="B4:AS5 B10:Q10 B9 B2:D2 F2:AS2 B8:F8 B7 D7:E7 H8:AS9 B6:D6 G6:AS6 D9:E9 B12:G12 C11:AS11 B16:AS17 C14:G14 B22:AS23 C19:Q19 B45:Q45 C43:AS43 B25:Q27 C24:G24 B44:H44 L44:N44 B42:AS42 B40:J40 L40:AS40 B36:AS36 B34:J34 L34:Q34 B20:J20 L20:AS20 C13:E13 G13:I13 I12:AS12 I14:Q14 B32:Q32 B31:G31 I31:Q31 B33:G33 I33:Q33 G7 I7:AS7 B18:E18 G18:H18 J18 L18:AS18 L13:M13 I24:AS24 B29:Q30 B28:J28 L28:AS28 B15:Q15 S14:AS15 S19:AS19 B21:Q21 S21:AS21 S25:AS27 S10:AS10 B35:Q35 S29:AS35 B37:Q39 S37:AS39 B41:Q41 S41:AS41 S45:AS45 J44 P44:R44 T44 W44:X44 AA44 AD44 AH44 AJ44 AM44:AN44 AP44:AR44 O13:T13 V13:X13 AC13:AS13 B3:O3 Q3:AC3 AE3:AS3">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="between">
+      <formula>1</formula>
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R34">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="between">
+      <formula>1</formula>
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
To run on laptop as well
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\heins\GitHub\Lists\scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="4656" yWindow="0" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="pairs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>&amp;</t>
   </si>
@@ -157,6 +152,21 @@
   </si>
   <si>
     <t>ks vs gz</t>
+  </si>
+  <si>
+    <t>A vs @</t>
+  </si>
+  <si>
+    <t>A vs (@)</t>
+  </si>
+  <si>
+    <t>s vs z</t>
+  </si>
+  <si>
+    <t>i vs I</t>
+  </si>
+  <si>
+    <t>@ vs -</t>
   </si>
 </sst>
 </file>
@@ -813,7 +823,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,6 +854,7 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -890,7 +901,7 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="8">
     <dxf>
       <font>
         <color auto="1"/>
@@ -928,206 +939,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1439,7 +1250,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1450,43 +1261,46 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AU49"/>
+  <dimension ref="A1:AU55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="35" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.28515625" customWidth="1"/>
-    <col min="40" max="41" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="19" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="35" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.33203125" customWidth="1"/>
+    <col min="40" max="41" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.33203125" customWidth="1"/>
     <col min="44" max="44" width="5" customWidth="1"/>
-    <col min="45" max="45" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" customWidth="1"/>
-    <col min="47" max="47" width="6.7109375" customWidth="1"/>
+    <col min="45" max="45" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.44140625" customWidth="1"/>
+    <col min="47" max="47" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1626,7 +1440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1916,7 +1730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2061,7 +1875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2206,7 +2020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2351,7 +2165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2641,7 +2455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2786,7 +2600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2931,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +2890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -3221,7 +3035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3366,7 +3180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -3511,7 +3325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -3656,7 +3470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3801,7 +3615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -3946,7 +3760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -4091,7 +3905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -4236,7 +4050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -4381,7 +4195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -4526,7 +4340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -4671,7 +4485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -4816,7 +4630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -4961,7 +4775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -5106,7 +4920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -5251,7 +5065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5396,7 +5210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -5541,7 +5355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -5686,7 +5500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -5831,7 +5645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -5976,7 +5790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -6121,7 +5935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -6266,7 +6080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -6411,7 +6225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -6556,7 +6370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -6701,7 +6515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -6846,7 +6660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -6991,7 +6805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -7136,7 +6950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -7281,7 +7095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -7426,7 +7240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -7571,7 +7385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -7716,7 +7530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
         <v>42</v>
       </c>
@@ -7861,7 +7675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -8006,7 +7820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="3">
         <f>SUM(B2:B45)</f>
         <v>34634</v>
@@ -8188,7 +8002,7 @@
         <v>1227046</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>44</v>
       </c>
@@ -8373,13 +8187,13 @@
         <v>438</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="AU48" s="14">
         <f>COUNTIF(A2:A45, "&lt;&gt;0")^2</f>
         <v>1936</v>
       </c>
     </row>
-    <row r="49" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -8388,40 +8202,70 @@
         <v>0.2262396694214876</v>
       </c>
     </row>
+    <row r="50" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B55" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B4:AS5 B10:Q10 B9 B2:D2 F2:AS2 B8:F8 B7 D7:E7 H8:AS9 B6:D6 G6:AS6 D9:E9 B12:G12 C11:AS11 B16:AS17 C14:G14 B22:AS23 C19:Q19 B45:Q45 C43:AS43 B25:Q27 C24:G24 B44:H44 L44:N44 B42:AS42 B40:J40 L40:AS40 B36:AS36 B34:J34 L34:Q34 B20:J20 L20:AS20 C13:E13 G13:I13 I12:AS12 I14:Q14 B32:Q32 B31:G31 I31:Q31 B33:G33 I33:Q33 G7 I7:AS7 B18:E18 G18:H18 J18 L18:AS18 L13:M13 I24:AS24 B29:Q30 B28:J28 L28:AS28 B15:Q15 S14:AS15 S19:AS19 B21:Q21 S21:AS21 S25:AS27 S10:AS10 B35:Q35 S29:AS35 B37:Q39 S37:AS39 B41:Q41 S41:AS41 S45:AS45 J44 P44:R44 T44 W44:X44 AA44 AD44 AH44 AJ44 AM44:AN44 AP44:AR44 O13:T13 V13:X13 AC13:AS13 B3:O3 Q3:AC3 AE3:AS3">
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R34">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed to new accepts format
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\heins\GitHub\Lists\scripts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4656" yWindow="0" windowWidth="19416" windowHeight="11016"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19410" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="pairs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -160,13 +165,13 @@
     <t>A vs (@)</t>
   </si>
   <si>
-    <t>s vs z</t>
-  </si>
-  <si>
     <t>i vs I</t>
   </si>
   <si>
     <t>@ vs -</t>
+  </si>
+  <si>
+    <t>s vs z, esp word end</t>
   </si>
 </sst>
 </file>
@@ -901,7 +906,87 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1250,7 +1335,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1267,40 +1352,40 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="35" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.33203125" customWidth="1"/>
-    <col min="40" max="41" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.33203125" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="35" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.28515625" customWidth="1"/>
+    <col min="40" max="41" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
     <col min="44" max="44" width="5" customWidth="1"/>
-    <col min="45" max="45" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.44140625" customWidth="1"/>
-    <col min="47" max="47" width="6.6640625" customWidth="1"/>
+    <col min="45" max="45" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" customWidth="1"/>
+    <col min="47" max="47" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1440,7 +1525,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="16">
-        <v>1829</v>
+        <v>1832</v>
       </c>
       <c r="L2" s="6">
         <v>0</v>
@@ -1490,7 +1575,7 @@
         <v>368</v>
       </c>
       <c r="Q2" s="6">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="R2" s="6">
         <v>0</v>
@@ -1538,7 +1623,7 @@
         <v>2949</v>
       </c>
       <c r="AG2" s="6">
-        <v>8290</v>
+        <v>8289</v>
       </c>
       <c r="AH2" s="6">
         <v>0</v>
@@ -1547,16 +1632,16 @@
         <v>1843</v>
       </c>
       <c r="AJ2" s="6">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="AK2" s="6">
         <v>4165</v>
       </c>
       <c r="AL2" s="6">
-        <v>2839</v>
+        <v>2841</v>
       </c>
       <c r="AM2" s="6">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AN2" s="6">
         <v>0</v>
@@ -1578,14 +1663,14 @@
       </c>
       <c r="AT2" s="3">
         <f>SUM(B2:AS2)</f>
-        <v>41456</v>
+        <v>41453</v>
       </c>
       <c r="AU2" s="3">
         <f>COUNTIF(B2:AS2, 0)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1625,14 +1710,14 @@
       <c r="M3" s="4">
         <v>0</v>
       </c>
-      <c r="N3" s="4">
-        <v>52</v>
+      <c r="N3" s="17">
+        <v>53</v>
       </c>
       <c r="O3" s="4">
         <v>0</v>
       </c>
       <c r="P3" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="4">
         <v>0</v>
@@ -1662,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="Z3" s="4">
-        <v>2092</v>
+        <v>2064</v>
       </c>
       <c r="AA3" s="4">
         <v>0</v>
@@ -1686,25 +1771,25 @@
         <v>0</v>
       </c>
       <c r="AH3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="4">
-        <v>10427</v>
+        <v>10440</v>
       </c>
       <c r="AK3" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AM3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3" s="4">
         <v>0</v>
@@ -1718,19 +1803,19 @@
       <c r="AR3" s="4">
         <v>0</v>
       </c>
-      <c r="AS3" s="9">
+      <c r="AS3" s="20">
         <v>4</v>
       </c>
       <c r="AT3" s="3">
         <f t="shared" ref="AT3:AT45" si="0">SUM(B3:AS3)</f>
-        <v>12594</v>
+        <v>12562</v>
       </c>
       <c r="AU3" s="3">
         <f t="shared" ref="AU3:AU45" si="1">COUNTIF(B3:AS3, 0)</f>
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1822,13 +1907,13 @@
         <v>2</v>
       </c>
       <c r="AE4" s="4">
-        <v>4319</v>
+        <v>4320</v>
       </c>
       <c r="AF4" s="4">
         <v>6</v>
       </c>
       <c r="AG4" s="4">
-        <v>2317</v>
+        <v>2318</v>
       </c>
       <c r="AH4" s="4">
         <v>0</v>
@@ -1837,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="4">
-        <v>795</v>
+        <v>806</v>
       </c>
       <c r="AK4" s="4">
         <v>0</v>
@@ -1868,14 +1953,14 @@
       </c>
       <c r="AT4" s="3">
         <f t="shared" si="0"/>
-        <v>7460</v>
+        <v>7473</v>
       </c>
       <c r="AU4" s="3">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1922,7 +2007,7 @@
         <v>631</v>
       </c>
       <c r="P5" s="4">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Q5" s="4">
         <v>0</v>
@@ -1952,7 +2037,7 @@
         <v>2766</v>
       </c>
       <c r="Z5" s="4">
-        <v>2122</v>
+        <v>2148</v>
       </c>
       <c r="AA5" s="4">
         <v>376</v>
@@ -1967,13 +2052,13 @@
         <v>4445</v>
       </c>
       <c r="AE5" s="4">
-        <v>20364</v>
+        <v>20363</v>
       </c>
       <c r="AF5" s="4">
         <v>10147</v>
       </c>
       <c r="AG5" s="4">
-        <v>29248</v>
+        <v>29246</v>
       </c>
       <c r="AH5" s="4">
         <v>2</v>
@@ -1982,13 +2067,13 @@
         <v>3163</v>
       </c>
       <c r="AJ5" s="4">
-        <v>31439</v>
+        <v>31430</v>
       </c>
       <c r="AK5" s="4">
-        <v>9055</v>
+        <v>9056</v>
       </c>
       <c r="AL5" s="4">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="AM5" s="4">
         <v>352</v>
@@ -1997,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="AO5" s="4">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="AP5" s="4">
         <v>303</v>
@@ -2013,14 +2098,14 @@
       </c>
       <c r="AT5" s="3">
         <f t="shared" si="0"/>
-        <v>131164</v>
+        <v>131180</v>
       </c>
       <c r="AU5" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2137,7 @@
         <v>18</v>
       </c>
       <c r="K6" s="17">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="L6" s="4">
         <v>11</v>
@@ -2097,7 +2182,7 @@
         <v>526</v>
       </c>
       <c r="Z6" s="4">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="AA6" s="4">
         <v>95</v>
@@ -2118,7 +2203,7 @@
         <v>2611</v>
       </c>
       <c r="AG6" s="4">
-        <v>6075</v>
+        <v>6072</v>
       </c>
       <c r="AH6" s="4">
         <v>24</v>
@@ -2130,10 +2215,10 @@
         <v>8865</v>
       </c>
       <c r="AK6" s="4">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="AL6" s="4">
-        <v>2791</v>
+        <v>2776</v>
       </c>
       <c r="AM6" s="4">
         <v>198</v>
@@ -2142,13 +2227,13 @@
         <v>27</v>
       </c>
       <c r="AO6" s="4">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AP6" s="4">
         <v>82</v>
       </c>
       <c r="AQ6" s="4">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AR6" s="4">
         <v>0</v>
@@ -2158,14 +2243,14 @@
       </c>
       <c r="AT6" s="3">
         <f t="shared" si="0"/>
-        <v>40156</v>
+        <v>40138</v>
       </c>
       <c r="AU6" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2263,7 +2348,7 @@
         <v>24</v>
       </c>
       <c r="AG7" s="4">
-        <v>2606</v>
+        <v>2609</v>
       </c>
       <c r="AH7" s="4">
         <v>0</v>
@@ -2278,7 +2363,7 @@
         <v>307</v>
       </c>
       <c r="AL7" s="4">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="AM7" s="4">
         <v>50</v>
@@ -2303,14 +2388,14 @@
       </c>
       <c r="AT7" s="3">
         <f t="shared" si="0"/>
-        <v>5869</v>
+        <v>5870</v>
       </c>
       <c r="AU7" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2455,7 +2540,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2496,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="4">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="O9" s="4">
         <v>552</v>
@@ -2553,7 +2638,7 @@
         <v>2001</v>
       </c>
       <c r="AG9" s="4">
-        <v>7583</v>
+        <v>7582</v>
       </c>
       <c r="AH9" s="4">
         <v>4</v>
@@ -2562,13 +2647,13 @@
         <v>1322</v>
       </c>
       <c r="AJ9" s="4">
-        <v>2704</v>
+        <v>2701</v>
       </c>
       <c r="AK9" s="4">
-        <v>5287</v>
+        <v>5288</v>
       </c>
       <c r="AL9" s="4">
-        <v>3120</v>
+        <v>3122</v>
       </c>
       <c r="AM9" s="4">
         <v>140</v>
@@ -2593,14 +2678,14 @@
       </c>
       <c r="AT9" s="3">
         <f t="shared" si="0"/>
-        <v>41326</v>
+        <v>41327</v>
       </c>
       <c r="AU9" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2698,7 +2783,7 @@
         <v>2880</v>
       </c>
       <c r="AG10" s="4">
-        <v>10343</v>
+        <v>10342</v>
       </c>
       <c r="AH10" s="4">
         <v>61</v>
@@ -2710,10 +2795,10 @@
         <v>1199</v>
       </c>
       <c r="AK10" s="4">
-        <v>10307</v>
+        <v>10306</v>
       </c>
       <c r="AL10" s="4">
-        <v>10260</v>
+        <v>10261</v>
       </c>
       <c r="AM10" s="4">
         <v>752</v>
@@ -2738,14 +2823,14 @@
       </c>
       <c r="AT10" s="3">
         <f t="shared" si="0"/>
-        <v>87371</v>
+        <v>87370</v>
       </c>
       <c r="AU10" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2843,7 +2928,7 @@
         <v>15</v>
       </c>
       <c r="AG11" s="4">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AH11" s="4">
         <v>8</v>
@@ -2883,14 +2968,14 @@
       </c>
       <c r="AT11" s="3">
         <f t="shared" si="0"/>
-        <v>5288</v>
+        <v>5291</v>
       </c>
       <c r="AU11" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2964,10 +3049,10 @@
         <v>1</v>
       </c>
       <c r="Y12" s="4">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="Z12" s="4">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AA12" s="4">
         <v>20</v>
@@ -2979,7 +3064,7 @@
         <v>47</v>
       </c>
       <c r="AD12" s="4">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AE12" s="4">
         <v>2421</v>
@@ -2991,19 +3076,19 @@
         <v>569</v>
       </c>
       <c r="AH12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" s="4">
         <v>67</v>
       </c>
       <c r="AJ12" s="4">
-        <v>5798</v>
+        <v>5861</v>
       </c>
       <c r="AK12" s="4">
         <v>1035</v>
       </c>
       <c r="AL12" s="4">
-        <v>1057</v>
+        <v>1075</v>
       </c>
       <c r="AM12" s="4">
         <v>15</v>
@@ -3028,14 +3113,14 @@
       </c>
       <c r="AT12" s="3">
         <f t="shared" si="0"/>
-        <v>15281</v>
+        <v>15358</v>
       </c>
       <c r="AU12" s="3">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3043,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -3061,7 +3146,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="17">
         <v>11</v>
@@ -3180,7 +3265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -3194,7 +3279,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="4">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="4">
         <v>331</v>
@@ -3284,7 +3369,7 @@
         <v>196</v>
       </c>
       <c r="AI14" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AJ14" s="4">
         <v>0</v>
@@ -3318,14 +3403,14 @@
       </c>
       <c r="AT14" s="3">
         <f t="shared" si="0"/>
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="AU14" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -3390,7 +3475,7 @@
         <v>36</v>
       </c>
       <c r="V15" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W15" s="4">
         <v>0</v>
@@ -3438,7 +3523,7 @@
         <v>4</v>
       </c>
       <c r="AL15" s="4">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AM15" s="4">
         <v>11</v>
@@ -3463,14 +3548,14 @@
       </c>
       <c r="AT15" s="3">
         <f t="shared" si="0"/>
-        <v>13725</v>
+        <v>13726</v>
       </c>
       <c r="AU15" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3478,13 +3563,13 @@
         <v>134</v>
       </c>
       <c r="C16" s="4">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="D16" s="4">
         <v>0</v>
       </c>
       <c r="E16" s="4">
-        <v>890</v>
+        <v>917</v>
       </c>
       <c r="F16" s="4">
         <v>169</v>
@@ -3595,7 +3680,7 @@
         <v>2</v>
       </c>
       <c r="AP16" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AQ16" s="4">
         <v>0</v>
@@ -3608,14 +3693,14 @@
       </c>
       <c r="AT16" s="3">
         <f t="shared" si="0"/>
-        <v>4892</v>
+        <v>4893</v>
       </c>
       <c r="AU16" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -3713,7 +3798,7 @@
         <v>289</v>
       </c>
       <c r="AG17" s="4">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AH17" s="4">
         <v>2</v>
@@ -3753,14 +3838,14 @@
       </c>
       <c r="AT17" s="3">
         <f t="shared" si="0"/>
-        <v>6737</v>
+        <v>6734</v>
       </c>
       <c r="AU17" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -3804,7 +3889,7 @@
         <v>28</v>
       </c>
       <c r="O18" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P18" s="4">
         <v>0</v>
@@ -3870,7 +3955,7 @@
         <v>0</v>
       </c>
       <c r="AK18" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AL18" s="4">
         <v>8</v>
@@ -3898,14 +3983,14 @@
       </c>
       <c r="AT18" s="3">
         <f t="shared" si="0"/>
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AU18" s="3">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -3922,7 +4007,7 @@
         <v>775</v>
       </c>
       <c r="F19" s="4">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -4043,14 +4128,14 @@
       </c>
       <c r="AT19" s="3">
         <f t="shared" si="0"/>
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="AU19" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -4195,12 +4280,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8">
-        <v>2928</v>
+        <v>2929</v>
       </c>
       <c r="C21" s="4">
         <v>1499</v>
@@ -4212,7 +4297,7 @@
         <v>6320</v>
       </c>
       <c r="F21" s="4">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="G21" s="4">
         <v>429</v>
@@ -4221,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="4">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="J21" s="4">
         <v>2436</v>
@@ -4333,14 +4418,14 @@
       </c>
       <c r="AT21" s="3">
         <f t="shared" si="0"/>
-        <v>34244</v>
+        <v>34243</v>
       </c>
       <c r="AU21" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -4348,7 +4433,7 @@
         <v>682</v>
       </c>
       <c r="C22" s="4">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D22" s="4">
         <v>1774</v>
@@ -4366,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="J22" s="4">
         <v>6717</v>
@@ -4485,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -4630,7 +4715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -4698,7 +4783,7 @@
         <v>1381</v>
       </c>
       <c r="W24" s="4">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="X24" s="4">
         <v>0</v>
@@ -4719,7 +4804,7 @@
         <v>21</v>
       </c>
       <c r="AD24" s="4">
-        <v>1990</v>
+        <v>1985</v>
       </c>
       <c r="AE24" s="4">
         <v>1982</v>
@@ -4740,7 +4825,7 @@
         <v>84</v>
       </c>
       <c r="AK24" s="4">
-        <v>1863</v>
+        <v>1868</v>
       </c>
       <c r="AL24" s="4">
         <v>4777</v>
@@ -4768,14 +4853,14 @@
       </c>
       <c r="AT24" s="3">
         <f t="shared" si="0"/>
-        <v>24026</v>
+        <v>24027</v>
       </c>
       <c r="AU24" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -4786,10 +4871,10 @@
         <v>949</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E25" s="4">
-        <v>3152</v>
+        <v>3142</v>
       </c>
       <c r="F25" s="4">
         <v>917</v>
@@ -4882,7 +4967,7 @@
         <v>9</v>
       </c>
       <c r="AJ25" s="4">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="AK25" s="4">
         <v>82</v>
@@ -4920,7 +5005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -4934,7 +5019,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="4">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="F26" s="4">
         <v>1244</v>
@@ -4973,7 +5058,7 @@
         <v>257</v>
       </c>
       <c r="R26" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S26" s="4">
         <v>10</v>
@@ -5006,7 +5091,7 @@
         <v>377</v>
       </c>
       <c r="AC26" s="4">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AD26" s="4">
         <v>4</v>
@@ -5027,7 +5112,7 @@
         <v>18</v>
       </c>
       <c r="AJ26" s="4">
-        <v>6722</v>
+        <v>6720</v>
       </c>
       <c r="AK26" s="4">
         <v>34</v>
@@ -5058,14 +5143,14 @@
       </c>
       <c r="AT26" s="3">
         <f t="shared" si="0"/>
-        <v>20757</v>
+        <v>20754</v>
       </c>
       <c r="AU26" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5073,7 +5158,7 @@
         <v>2134</v>
       </c>
       <c r="C27" s="4">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -5151,7 +5236,7 @@
         <v>850</v>
       </c>
       <c r="AC27" s="4">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AD27" s="4">
         <v>0</v>
@@ -5190,7 +5275,7 @@
         <v>2</v>
       </c>
       <c r="AP27" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AQ27" s="4">
         <v>0</v>
@@ -5203,14 +5288,14 @@
       </c>
       <c r="AT27" s="3">
         <f t="shared" si="0"/>
-        <v>13711</v>
+        <v>13710</v>
       </c>
       <c r="AU27" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -5227,7 +5312,7 @@
         <v>7521</v>
       </c>
       <c r="F28" s="4">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G28" s="4">
         <v>3</v>
@@ -5236,7 +5321,7 @@
         <v>127</v>
       </c>
       <c r="I28" s="4">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J28" s="4">
         <v>398</v>
@@ -5308,7 +5393,7 @@
         <v>1511</v>
       </c>
       <c r="AG28" s="4">
-        <v>3603</v>
+        <v>3604</v>
       </c>
       <c r="AH28" s="4">
         <v>766</v>
@@ -5323,7 +5408,7 @@
         <v>1348</v>
       </c>
       <c r="AL28" s="4">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="AM28" s="4">
         <v>426</v>
@@ -5348,14 +5433,14 @@
       </c>
       <c r="AT28" s="3">
         <f t="shared" si="0"/>
-        <v>34838</v>
+        <v>34835</v>
       </c>
       <c r="AU28" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -5369,7 +5454,7 @@
         <v>50</v>
       </c>
       <c r="E29" s="4">
-        <v>2678</v>
+        <v>2679</v>
       </c>
       <c r="F29" s="4">
         <v>669</v>
@@ -5381,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="4">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="J29" s="4">
         <v>49</v>
@@ -5465,7 +5550,7 @@
         <v>2</v>
       </c>
       <c r="AK29" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL29" s="4">
         <v>6</v>
@@ -5474,7 +5559,7 @@
         <v>5</v>
       </c>
       <c r="AN29" s="4">
-        <v>3494</v>
+        <v>3495</v>
       </c>
       <c r="AO29" s="4">
         <v>3</v>
@@ -5493,14 +5578,14 @@
       </c>
       <c r="AT29" s="3">
         <f t="shared" si="0"/>
-        <v>9484</v>
+        <v>9487</v>
       </c>
       <c r="AU29" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -5610,7 +5695,7 @@
         <v>4759</v>
       </c>
       <c r="AK30" s="4">
-        <v>5038</v>
+        <v>5037</v>
       </c>
       <c r="AL30" s="4">
         <v>3870</v>
@@ -5638,14 +5723,14 @@
       </c>
       <c r="AT30" s="3">
         <f t="shared" si="0"/>
-        <v>59450</v>
+        <v>59449</v>
       </c>
       <c r="AU30" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -5659,7 +5744,7 @@
         <v>19</v>
       </c>
       <c r="E31" s="4">
-        <v>9653</v>
+        <v>9655</v>
       </c>
       <c r="F31" s="4">
         <v>2769</v>
@@ -5674,7 +5759,7 @@
         <v>3128</v>
       </c>
       <c r="J31" s="4">
-        <v>8755</v>
+        <v>8753</v>
       </c>
       <c r="K31" s="4">
         <v>0</v>
@@ -5728,10 +5813,10 @@
         <v>112</v>
       </c>
       <c r="AB31" s="4">
-        <v>9089</v>
+        <v>9088</v>
       </c>
       <c r="AC31" s="4">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="AD31" s="4">
         <v>728</v>
@@ -5790,7 +5875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -5819,7 +5904,7 @@
         <v>2475</v>
       </c>
       <c r="J32" s="4">
-        <v>4262</v>
+        <v>4261</v>
       </c>
       <c r="K32" s="4">
         <v>0</v>
@@ -5873,7 +5958,7 @@
         <v>29</v>
       </c>
       <c r="AB32" s="4">
-        <v>2259</v>
+        <v>2260</v>
       </c>
       <c r="AC32" s="4">
         <v>774</v>
@@ -5935,7 +6020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -5952,7 +6037,7 @@
         <v>6140</v>
       </c>
       <c r="F33" s="4">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="G33" s="4">
         <v>101</v>
@@ -5970,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="4">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M33" s="4">
         <v>114</v>
@@ -6006,7 +6091,7 @@
         <v>1350</v>
       </c>
       <c r="X33" s="4">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="Y33" s="4">
         <v>871</v>
@@ -6048,7 +6133,7 @@
         <v>5622</v>
       </c>
       <c r="AL33" s="4">
-        <v>11874</v>
+        <v>11872</v>
       </c>
       <c r="AM33" s="4">
         <v>773</v>
@@ -6073,14 +6158,14 @@
       </c>
       <c r="AT33" s="3">
         <f t="shared" si="0"/>
-        <v>65945</v>
+        <v>65939</v>
       </c>
       <c r="AU33" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -6136,7 +6221,7 @@
         <v>0</v>
       </c>
       <c r="S34" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T34" s="4">
         <v>29</v>
@@ -6187,13 +6272,13 @@
         <v>1184</v>
       </c>
       <c r="AJ34" s="4">
-        <v>4900</v>
+        <v>4839</v>
       </c>
       <c r="AK34" s="4">
         <v>1876</v>
       </c>
       <c r="AL34" s="4">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="AM34" s="4">
         <v>127</v>
@@ -6218,14 +6303,14 @@
       </c>
       <c r="AT34" s="3">
         <f t="shared" si="0"/>
-        <v>26166</v>
+        <v>26105</v>
       </c>
       <c r="AU34" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -6233,7 +6318,7 @@
         <v>2165</v>
       </c>
       <c r="C35" s="4">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D35" s="4">
         <v>6</v>
@@ -6254,7 +6339,7 @@
         <v>1895</v>
       </c>
       <c r="J35" s="4">
-        <v>3333</v>
+        <v>3334</v>
       </c>
       <c r="K35" s="4">
         <v>0</v>
@@ -6266,7 +6351,7 @@
         <v>464</v>
       </c>
       <c r="N35" s="4">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O35" s="4">
         <v>221</v>
@@ -6296,7 +6381,7 @@
         <v>7</v>
       </c>
       <c r="X35" s="4">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Y35" s="4">
         <v>57</v>
@@ -6308,7 +6393,7 @@
         <v>40</v>
       </c>
       <c r="AB35" s="4">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AC35" s="4">
         <v>449</v>
@@ -6332,7 +6417,7 @@
         <v>11</v>
       </c>
       <c r="AJ35" s="4">
-        <v>4976</v>
+        <v>4978</v>
       </c>
       <c r="AK35" s="4">
         <v>578</v>
@@ -6370,12 +6455,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="8">
-        <v>5470</v>
+        <v>5471</v>
       </c>
       <c r="C36" s="4">
         <v>151</v>
@@ -6384,10 +6469,10 @@
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <v>11769</v>
+        <v>11771</v>
       </c>
       <c r="F36" s="4">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="G36" s="4">
         <v>1101</v>
@@ -6399,13 +6484,13 @@
         <v>4427</v>
       </c>
       <c r="J36" s="4">
-        <v>10741</v>
+        <v>10740</v>
       </c>
       <c r="K36" s="4">
         <v>0</v>
       </c>
       <c r="L36" s="4">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="M36" s="4">
         <v>268</v>
@@ -6417,7 +6502,7 @@
         <v>406</v>
       </c>
       <c r="P36" s="4">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="Q36" s="4">
         <v>197</v>
@@ -6453,10 +6538,10 @@
         <v>180</v>
       </c>
       <c r="AB36" s="4">
-        <v>12087</v>
+        <v>12086</v>
       </c>
       <c r="AC36" s="4">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AD36" s="4">
         <v>2771</v>
@@ -6471,19 +6556,19 @@
         <v>3199</v>
       </c>
       <c r="AH36" s="4">
-        <v>4621</v>
+        <v>4622</v>
       </c>
       <c r="AI36" s="4">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="AJ36" s="4">
         <v>58</v>
       </c>
       <c r="AK36" s="4">
-        <v>2495</v>
+        <v>2499</v>
       </c>
       <c r="AL36" s="4">
-        <v>3879</v>
+        <v>3884</v>
       </c>
       <c r="AM36" s="4">
         <v>579</v>
@@ -6508,19 +6593,19 @@
       </c>
       <c r="AT36" s="3">
         <f t="shared" si="0"/>
-        <v>95708</v>
+        <v>95721</v>
       </c>
       <c r="AU36" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="8">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="C37" s="4">
         <v>937</v>
@@ -6529,13 +6614,13 @@
         <v>2</v>
       </c>
       <c r="E37" s="4">
-        <v>6828</v>
+        <v>6827</v>
       </c>
       <c r="F37" s="4">
         <v>1186</v>
       </c>
       <c r="G37" s="4">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H37" s="17">
         <v>0</v>
@@ -6544,13 +6629,13 @@
         <v>4848</v>
       </c>
       <c r="J37" s="4">
-        <v>7113</v>
+        <v>7114</v>
       </c>
       <c r="K37" s="4">
         <v>0</v>
       </c>
       <c r="L37" s="4">
-        <v>927</v>
+        <v>988</v>
       </c>
       <c r="M37" s="4">
         <v>78</v>
@@ -6616,7 +6701,7 @@
         <v>1120</v>
       </c>
       <c r="AH37" s="4">
-        <v>1322</v>
+        <v>1261</v>
       </c>
       <c r="AI37" s="4">
         <v>4495</v>
@@ -6628,7 +6713,7 @@
         <v>60</v>
       </c>
       <c r="AL37" s="4">
-        <v>16209</v>
+        <v>16208</v>
       </c>
       <c r="AM37" s="4">
         <v>262</v>
@@ -6653,14 +6738,14 @@
       </c>
       <c r="AT37" s="3">
         <f t="shared" si="0"/>
-        <v>65349</v>
+        <v>65348</v>
       </c>
       <c r="AU37" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -6671,13 +6756,13 @@
         <v>1259</v>
       </c>
       <c r="D38" s="4">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="E38" s="4">
-        <v>13056</v>
+        <v>13053</v>
       </c>
       <c r="F38" s="4">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="G38" s="4">
         <v>291</v>
@@ -6686,10 +6771,10 @@
         <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="J38" s="4">
-        <v>10637</v>
+        <v>10638</v>
       </c>
       <c r="K38" s="4">
         <v>0</v>
@@ -6704,7 +6789,7 @@
         <v>121</v>
       </c>
       <c r="O38" s="4">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="P38" s="4">
         <v>26</v>
@@ -6740,7 +6825,7 @@
         <v>64</v>
       </c>
       <c r="AA38" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB38" s="4">
         <v>5220</v>
@@ -6761,13 +6846,13 @@
         <v>285</v>
       </c>
       <c r="AH38" s="4">
-        <v>2936</v>
+        <v>2937</v>
       </c>
       <c r="AI38" s="4">
         <v>95</v>
       </c>
       <c r="AJ38" s="4">
-        <v>9070</v>
+        <v>9069</v>
       </c>
       <c r="AK38" s="4">
         <v>967</v>
@@ -6798,14 +6883,14 @@
       </c>
       <c r="AT38" s="3">
         <f t="shared" si="0"/>
-        <v>65279</v>
+        <v>65278</v>
       </c>
       <c r="AU38" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -6918,7 +7003,7 @@
         <v>4</v>
       </c>
       <c r="AL39" s="4">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AM39" s="4">
         <v>1</v>
@@ -6943,14 +7028,14 @@
       </c>
       <c r="AT39" s="3">
         <f t="shared" si="0"/>
-        <v>5430</v>
+        <v>5428</v>
       </c>
       <c r="AU39" s="3">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -7095,7 +7180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -7240,7 +7325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -7385,7 +7470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -7530,7 +7615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>42</v>
       </c>
@@ -7675,7 +7760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -7820,30 +7905,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="3">
         <f>SUM(B2:B45)</f>
-        <v>34634</v>
+        <v>34633</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" ref="C46:AT46" si="2">SUM(C2:C45)</f>
-        <v>11668</v>
+        <v>11636</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" si="2"/>
-        <v>7547</v>
+        <v>7560</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" si="2"/>
-        <v>131510</v>
+        <v>131525</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="2"/>
-        <v>38321</v>
+        <v>38314</v>
       </c>
       <c r="G46" s="3">
         <f t="shared" si="2"/>
-        <v>5296</v>
+        <v>5299</v>
       </c>
       <c r="H46" s="3">
         <f t="shared" si="2"/>
@@ -7851,19 +7936,19 @@
       </c>
       <c r="I46" s="3">
         <f t="shared" si="2"/>
-        <v>37493</v>
+        <v>37494</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" si="2"/>
-        <v>79309</v>
+        <v>79308</v>
       </c>
       <c r="K46" s="3">
         <f t="shared" si="2"/>
-        <v>14128</v>
+        <v>14133</v>
       </c>
       <c r="L46" s="3">
         <f t="shared" si="2"/>
-        <v>14078</v>
+        <v>14137</v>
       </c>
       <c r="M46" s="3">
         <f t="shared" si="2"/>
@@ -7871,27 +7956,27 @@
       </c>
       <c r="N46" s="3">
         <f t="shared" si="2"/>
-        <v>2768</v>
+        <v>2769</v>
       </c>
       <c r="O46" s="3">
         <f t="shared" si="2"/>
-        <v>12336</v>
+        <v>12337</v>
       </c>
       <c r="P46" s="3">
         <f t="shared" si="2"/>
-        <v>4782</v>
+        <v>4783</v>
       </c>
       <c r="Q46" s="3">
         <f t="shared" si="2"/>
-        <v>6804</v>
+        <v>6801</v>
       </c>
       <c r="R46" s="3">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S46" s="3">
         <f t="shared" si="2"/>
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="T46" s="3">
         <f t="shared" si="2"/>
@@ -7903,11 +7988,11 @@
       </c>
       <c r="V46" s="3">
         <f t="shared" si="2"/>
-        <v>41260</v>
+        <v>41259</v>
       </c>
       <c r="W46" s="3">
         <f t="shared" si="2"/>
-        <v>8411</v>
+        <v>8412</v>
       </c>
       <c r="X46" s="3">
         <f t="shared" si="2"/>
@@ -7915,27 +8000,27 @@
       </c>
       <c r="Y46" s="3">
         <f t="shared" si="2"/>
-        <v>15574</v>
+        <v>15573</v>
       </c>
       <c r="Z46" s="3">
         <f t="shared" si="2"/>
-        <v>13856</v>
+        <v>13855</v>
       </c>
       <c r="AA46" s="3">
         <f t="shared" si="2"/>
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="AB46" s="3">
         <f t="shared" si="2"/>
-        <v>57474</v>
+        <v>57472</v>
       </c>
       <c r="AC46" s="3">
         <f t="shared" si="2"/>
-        <v>7435</v>
+        <v>7438</v>
       </c>
       <c r="AD46" s="3">
         <f t="shared" si="2"/>
-        <v>49930</v>
+        <v>49924</v>
       </c>
       <c r="AE46" s="3">
         <f t="shared" si="2"/>
@@ -7947,11 +8032,11 @@
       </c>
       <c r="AG46" s="3">
         <f t="shared" si="2"/>
-        <v>88674</v>
+        <v>88671</v>
       </c>
       <c r="AH46" s="3">
         <f t="shared" si="2"/>
-        <v>30110</v>
+        <v>30049</v>
       </c>
       <c r="AI46" s="3">
         <f t="shared" si="2"/>
@@ -7959,19 +8044,19 @@
       </c>
       <c r="AJ46" s="3">
         <f t="shared" si="2"/>
-        <v>109775</v>
+        <v>109785</v>
       </c>
       <c r="AK46" s="3">
         <f t="shared" si="2"/>
-        <v>57250</v>
+        <v>57254</v>
       </c>
       <c r="AL46" s="3">
         <f t="shared" si="2"/>
-        <v>82368</v>
+        <v>82366</v>
       </c>
       <c r="AM46" s="3">
         <f t="shared" si="2"/>
-        <v>4964</v>
+        <v>4961</v>
       </c>
       <c r="AN46" s="3">
         <f t="shared" si="2"/>
@@ -7987,7 +8072,7 @@
       </c>
       <c r="AQ46" s="3">
         <f t="shared" si="2"/>
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AR46" s="3">
         <f t="shared" si="2"/>
@@ -7999,10 +8084,10 @@
       </c>
       <c r="AT46" s="12">
         <f t="shared" si="2"/>
-        <v>1227046</v>
+        <v>1227038</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>44</v>
       </c>
@@ -8012,7 +8097,7 @@
       </c>
       <c r="C47" s="3">
         <f t="shared" ref="C47:AS47" si="3">COUNTIF(C2:C45, 0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" si="3"/>
@@ -8036,7 +8121,7 @@
       </c>
       <c r="I47" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J47" s="3">
         <f t="shared" si="3"/>
@@ -8064,7 +8149,7 @@
       </c>
       <c r="P47" s="3">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q47" s="3">
         <f t="shared" si="3"/>
@@ -8136,11 +8221,11 @@
       </c>
       <c r="AH47" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AI47" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AJ47" s="3">
         <f t="shared" si="3"/>
@@ -8148,19 +8233,19 @@
       </c>
       <c r="AK47" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL47" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM47" s="3">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AN47" s="3">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AO47" s="3">
         <f t="shared" si="3"/>
@@ -8184,88 +8269,88 @@
       </c>
       <c r="AU47" s="14">
         <f>SUM(AU2:AU45)</f>
-        <v>438</v>
+        <v>446</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="AU48" s="14">
         <f>COUNTIF(A2:A45, "&lt;&gt;0")^2</f>
         <v>1936</v>
       </c>
     </row>
-    <row r="49" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>45</v>
       </c>
       <c r="AU49" s="23">
         <f>AU47/AU48</f>
-        <v>0.2262396694214876</v>
+        <v>0.23037190082644629</v>
       </c>
     </row>
-    <row r="50" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="2:47" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+    <row r="55" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B55" s="24" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="2:47" x14ac:dyDescent="0.3">
-      <c r="B55" s="24" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:AS5 B10:Q10 B9 B2:D2 F2:AS2 B8:F8 B7 D7:E7 H8:AS9 B6:D6 G6:AS6 D9:E9 B12:G12 C11:AS11 B16:AS17 C14:G14 B22:AS23 C19:Q19 B45:Q45 C43:AS43 B25:Q27 C24:G24 B44:H44 L44:N44 B42:AS42 B40:J40 L40:AS40 B36:AS36 B34:J34 L34:Q34 B20:J20 L20:AS20 C13:E13 G13:I13 I12:AS12 I14:Q14 B32:Q32 B31:G31 I31:Q31 B33:G33 I33:Q33 G7 I7:AS7 B18:E18 G18:H18 J18 L18:AS18 L13:M13 I24:AS24 B29:Q30 B28:J28 L28:AS28 B15:Q15 S14:AS15 S19:AS19 B21:Q21 S21:AS21 S25:AS27 S10:AS10 B35:Q35 S29:AS35 B37:Q39 S37:AS39 B41:Q41 S41:AS41 S45:AS45 J44 P44:R44 T44 W44:X44 AA44 AD44 AH44 AJ44 AM44:AN44 AP44:AR44 O13:T13 V13:X13 AC13:AS13 B3:O3 Q3:AC3 AE3:AS3">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+  <conditionalFormatting sqref="B4:AS5 B10:Q10 B9 B2:D2 F2:AS2 B8:F8 B7 D7:E7 H8:AS9 B6:D6 G6:AS6 D9:E9 B12:G12 C11:AS11 B16:AS17 C14:G14 B22:AS23 C19:Q19 B45:Q45 C43:AS43 B25:Q27 C24:G24 B44:H44 L44:N44 B42:AS42 B40:J40 L40:AS40 B36:AS36 B34:J34 L34:Q34 B20:J20 L20:AS20 C13:E13 G13:I13 I12:AS12 I14:Q14 B32:Q32 B31:G31 I31:Q31 B33:G33 I33:Q33 G7 I7:AS7 B18:E18 G18:H18 J18 L18:AS18 L13:M13 I24:AS24 B29:Q30 B28:J28 L28:AS28 B15:Q15 S14:AS15 S19:AS19 B21:Q21 S21:AS21 S25:AS27 S10:AS10 B35:Q35 S29:AS35 B37:Q39 S37:AS39 B41:Q41 S41:AS41 S45:AS45 J44 P44:R44 T44 W44:X44 AA44 AD44 AH44 AJ44 AM44:AN44 AP44:AR44 O13:T13 V13:X13 AC13:AS13 B3:O3 Q3:AC3 AE3:AR3">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R34">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
       <formula>1</formula>
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>